<commit_message>
Monsterdatabase hele keten incl. Tonen in webapp
</commit_message>
<xml_diff>
--- a/data/wasstraat_config/Wasstraat_Config_HarmonizeV3.xlsx
+++ b/data/wasstraat_config/Wasstraat_Config_HarmonizeV3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjen/Dropbox/Development/wasstraat_archeologische_data/data/wasstraat_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10D9888-84F3-7A41-93F0-04BA1A8F4888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D553D1-FFDD-434C-95E1-10D88D974596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7820" yWindow="-28800" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Objecten" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="650">
   <si>
     <t>Object</t>
   </si>
@@ -2030,6 +2030,15 @@
   </si>
   <si>
     <t>["Monster_botanie.*"]</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>['PROJECT']</t>
+  </si>
+  <si>
+    <t>Om de projectnamen te kunnen matchen</t>
   </si>
 </sst>
 </file>
@@ -2471,7 +2480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
+    <sheetView zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -4938,10 +4947,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3BE5099-14EB-8E48-A984-D6BE092CC4FE}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection sqref="A1:XFD6"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5113,6 +5122,20 @@
       </c>
       <c r="C15" t="s">
         <v>632</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>647</v>
+      </c>
+      <c r="C16" t="s">
+        <v>648</v>
+      </c>
+      <c r="D16" t="s">
+        <v>649</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Verbeterde koppeling Foto's aan artefact
</commit_message>
<xml_diff>
--- a/data/wasstraat_config/Wasstraat_Config_HarmonizeV3.xlsx
+++ b/data/wasstraat_config/Wasstraat_Config_HarmonizeV3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjen/Dropbox/Development/wasstraat_archeologische_data/data/wasstraat_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DFBDDD-138A-B341-B2D7-C87DA0595FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C093040E-F751-FF4C-8FAD-448A5C3B711D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Objecten" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="897">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="898">
   <si>
     <t>Object</t>
   </si>
@@ -2796,6 +2796,9 @@
   </si>
   <si>
     <t>["DANlijst", "DARlijst"]</t>
+  </si>
+  <si>
+    <t>https://data.cultureelerfgoed.nl/term/id/abr/9084ba17-eefe-44db-8eab-d7b746668d9b</t>
   </si>
 </sst>
 </file>
@@ -3300,8 +3303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3629,7 +3632,7 @@
         <v>858</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>857</v>
+        <v>897</v>
       </c>
       <c r="H21" t="s">
         <v>588</v>
@@ -3835,16 +3838,16 @@
     <hyperlink ref="F18" r:id="rId9" xr:uid="{4C709E94-2D4A-2E47-8572-1F20FB605A51}"/>
     <hyperlink ref="F19" r:id="rId10" xr:uid="{BFFA1E12-134F-774E-8411-509A3441D5DD}"/>
     <hyperlink ref="F20" r:id="rId11" xr:uid="{7E596272-A81D-BF47-8BB2-35CE3CC2A65D}"/>
-    <hyperlink ref="F21" r:id="rId12" xr:uid="{8D820533-C636-9D4A-AE3D-39E4692FD2B4}"/>
-    <hyperlink ref="F23" r:id="rId13" xr:uid="{A1C8D6E1-4522-9949-B2BA-FCBDD0C63A32}"/>
-    <hyperlink ref="G14" r:id="rId14" xr:uid="{72E12E3E-5913-C84A-8E31-C85C99FBD593}"/>
-    <hyperlink ref="G15" r:id="rId15" xr:uid="{C064080B-0DC7-2C42-9E27-458ABB5BB9E7}"/>
-    <hyperlink ref="G21" r:id="rId16" xr:uid="{804ED6BF-97D8-894F-B3A6-1771ADB1A6F0}"/>
-    <hyperlink ref="G22" r:id="rId17" xr:uid="{4D12CAF9-7415-A248-9FCE-17BACDDBBD90}"/>
-    <hyperlink ref="G23" r:id="rId18" xr:uid="{B751360D-E2A6-8945-BBF7-7B891BAAA881}"/>
-    <hyperlink ref="G24" r:id="rId19" xr:uid="{783040BA-D699-BE4D-88BC-55B3819C2E2B}"/>
-    <hyperlink ref="G27" r:id="rId20" xr:uid="{4ED51761-89CD-FA43-A2DB-3F57DE3640E3}"/>
-    <hyperlink ref="G25" r:id="rId21" xr:uid="{42E53C2C-9279-3F4E-A141-C97807584DAD}"/>
+    <hyperlink ref="F23" r:id="rId12" xr:uid="{A1C8D6E1-4522-9949-B2BA-FCBDD0C63A32}"/>
+    <hyperlink ref="G14" r:id="rId13" xr:uid="{72E12E3E-5913-C84A-8E31-C85C99FBD593}"/>
+    <hyperlink ref="G15" r:id="rId14" xr:uid="{C064080B-0DC7-2C42-9E27-458ABB5BB9E7}"/>
+    <hyperlink ref="G21" r:id="rId15" xr:uid="{804ED6BF-97D8-894F-B3A6-1771ADB1A6F0}"/>
+    <hyperlink ref="G22" r:id="rId16" xr:uid="{4D12CAF9-7415-A248-9FCE-17BACDDBBD90}"/>
+    <hyperlink ref="G23" r:id="rId17" xr:uid="{B751360D-E2A6-8945-BBF7-7B891BAAA881}"/>
+    <hyperlink ref="G24" r:id="rId18" xr:uid="{783040BA-D699-BE4D-88BC-55B3819C2E2B}"/>
+    <hyperlink ref="G27" r:id="rId19" xr:uid="{4ED51761-89CD-FA43-A2DB-3F57DE3640E3}"/>
+    <hyperlink ref="G25" r:id="rId20" xr:uid="{42E53C2C-9279-3F4E-A141-C97807584DAD}"/>
+    <hyperlink ref="F21" r:id="rId21" xr:uid="{087416B1-3D05-8C4B-8A4C-B8850620DE7D}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId22"/>

</xml_diff>

<commit_message>
Monsters ingedeeld volgens wensen Steven
</commit_message>
<xml_diff>
--- a/data/wasstraat_config/Wasstraat_Config_HarmonizeV3.xlsx
+++ b/data/wasstraat_config/Wasstraat_Config_HarmonizeV3.xlsx
@@ -1,46 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjen/Dropbox/Development/wasstraat_archeologische_data/data/wasstraat_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD19592-BADD-2144-BE77-C444EA517A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33AAA364-7237-D44E-923F-0C378335F892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="760" windowWidth="26700" windowHeight="18880" firstSheet="1" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11240" yWindow="-28800" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Objecten" sheetId="1" r:id="rId1"/>
-    <sheet name="Rapport" sheetId="30" r:id="rId2"/>
-    <sheet name="Monster" sheetId="25" r:id="rId3"/>
-    <sheet name="ABR" sheetId="29" r:id="rId4"/>
-    <sheet name="Tekening" sheetId="28" r:id="rId5"/>
-    <sheet name="Monster_Schelp" sheetId="27" r:id="rId6"/>
-    <sheet name="Monster_Botanie" sheetId="26" r:id="rId7"/>
-    <sheet name="Put" sheetId="2" r:id="rId8"/>
-    <sheet name="Vlak" sheetId="3" r:id="rId9"/>
-    <sheet name="Spoor" sheetId="4" r:id="rId10"/>
-    <sheet name="Vulling" sheetId="5" r:id="rId11"/>
-    <sheet name="Vondst" sheetId="6" r:id="rId12"/>
-    <sheet name="Stelling" sheetId="7" r:id="rId13"/>
-    <sheet name="Artefact" sheetId="8" r:id="rId14"/>
-    <sheet name="Menselijk_Bot" sheetId="10" r:id="rId15"/>
-    <sheet name="Metaal" sheetId="11" r:id="rId16"/>
-    <sheet name="Munt" sheetId="12" r:id="rId17"/>
-    <sheet name="Schelp" sheetId="13" r:id="rId18"/>
-    <sheet name="Steen" sheetId="14" r:id="rId19"/>
-    <sheet name="Textiel" sheetId="15" r:id="rId20"/>
-    <sheet name="Dierlijk_Bot" sheetId="16" r:id="rId21"/>
-    <sheet name="Aardewerk" sheetId="17" r:id="rId22"/>
-    <sheet name="Glas" sheetId="18" r:id="rId23"/>
-    <sheet name="Hout" sheetId="19" r:id="rId24"/>
-    <sheet name="Bouwaardewerk" sheetId="21" r:id="rId25"/>
-    <sheet name="Leer" sheetId="22" r:id="rId26"/>
-    <sheet name="Fotobeschrijving" sheetId="23" r:id="rId27"/>
-    <sheet name="Fotokoppel" sheetId="24" r:id="rId28"/>
+    <sheet name="DT_Soort_Plant" sheetId="31" r:id="rId2"/>
+    <sheet name="DT_Soort_Schelp" sheetId="32" r:id="rId3"/>
+    <sheet name="DT_Soort_Deel" sheetId="33" r:id="rId4"/>
+    <sheet name="DT_Soort_Staat" sheetId="34" r:id="rId5"/>
+    <sheet name="Rapport" sheetId="30" r:id="rId6"/>
+    <sheet name="Monster" sheetId="25" r:id="rId7"/>
+    <sheet name="ABR" sheetId="29" r:id="rId8"/>
+    <sheet name="Tekening" sheetId="28" r:id="rId9"/>
+    <sheet name="Monster_Schelp" sheetId="27" r:id="rId10"/>
+    <sheet name="Monster_Botanie" sheetId="26" r:id="rId11"/>
+    <sheet name="Put" sheetId="2" r:id="rId12"/>
+    <sheet name="Vlak" sheetId="3" r:id="rId13"/>
+    <sheet name="Spoor" sheetId="4" r:id="rId14"/>
+    <sheet name="Vulling" sheetId="5" r:id="rId15"/>
+    <sheet name="Vondst" sheetId="6" r:id="rId16"/>
+    <sheet name="Stelling" sheetId="7" r:id="rId17"/>
+    <sheet name="Artefact" sheetId="8" r:id="rId18"/>
+    <sheet name="Menselijk_Bot" sheetId="10" r:id="rId19"/>
+    <sheet name="Metaal" sheetId="11" r:id="rId20"/>
+    <sheet name="Munt" sheetId="12" r:id="rId21"/>
+    <sheet name="Schelp" sheetId="13" r:id="rId22"/>
+    <sheet name="Steen" sheetId="14" r:id="rId23"/>
+    <sheet name="Textiel" sheetId="15" r:id="rId24"/>
+    <sheet name="Dierlijk_Bot" sheetId="16" r:id="rId25"/>
+    <sheet name="Aardewerk" sheetId="17" r:id="rId26"/>
+    <sheet name="Glas" sheetId="18" r:id="rId27"/>
+    <sheet name="Hout" sheetId="19" r:id="rId28"/>
+    <sheet name="Bouwaardewerk" sheetId="21" r:id="rId29"/>
+    <sheet name="Leer" sheetId="22" r:id="rId30"/>
+    <sheet name="Fotobeschrijving" sheetId="23" r:id="rId31"/>
+    <sheet name="Fotokoppel" sheetId="24" r:id="rId32"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -105,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="924">
   <si>
     <t>Object</t>
   </si>
@@ -1982,9 +1986,6 @@
     <t>["Monster_gegevens", "Monster_waardering"]</t>
   </si>
   <si>
-    <t>soort</t>
-  </si>
-  <si>
     <t>['SOORT']</t>
   </si>
   <si>
@@ -2012,15 +2013,9 @@
     <t>Monster_Schelp</t>
   </si>
   <si>
-    <t>["Monster_schelp.*"]</t>
-  </si>
-  <si>
     <t>Monster_Botanie</t>
   </si>
   <si>
-    <t>["Monster_botanie.*"]</t>
-  </si>
-  <si>
     <t>project</t>
   </si>
   <si>
@@ -2799,6 +2794,93 @@
   </si>
   <si>
     <t>['TOTAANTAL', 'AANTAL', '4b1', 'aant']</t>
+  </si>
+  <si>
+    <t>soort_botanie</t>
+  </si>
+  <si>
+    <t>soort_schelp</t>
+  </si>
+  <si>
+    <t>DT_Soort_Deel</t>
+  </si>
+  <si>
+    <t>DT_Soort_Plant</t>
+  </si>
+  <si>
+    <t>DT_Soort_Schelp</t>
+  </si>
+  <si>
+    <t>DT_Soort_Staat</t>
+  </si>
+  <si>
+    <t>["SPEC"]</t>
+  </si>
+  <si>
+    <t>oude_naam</t>
+  </si>
+  <si>
+    <t>wetenschappelijke_naam</t>
+  </si>
+  <si>
+    <t>nederlandse_naam</t>
+  </si>
+  <si>
+    <t>["CODENAAM"]</t>
+  </si>
+  <si>
+    <t>["NAAM NEDERLANDS"]</t>
+  </si>
+  <si>
+    <t>milieu</t>
+  </si>
+  <si>
+    <t>["MILIEU"]</t>
+  </si>
+  <si>
+    <t>["DEEL"]</t>
+  </si>
+  <si>
+    <t>["OMSCHRIJVING"]</t>
+  </si>
+  <si>
+    <t>uitleg</t>
+  </si>
+  <si>
+    <t>["UITLEG"]</t>
+  </si>
+  <si>
+    <t>["STAAT"]</t>
+  </si>
+  <si>
+    <t>["NAAM LATIJN"]</t>
+  </si>
+  <si>
+    <t>["WETENSCHAPPELIJKE NAAM"]</t>
+  </si>
+  <si>
+    <t>["OUDE NAAM"]</t>
+  </si>
+  <si>
+    <t>["NEDERLANDSE NAAM"]</t>
+  </si>
+  <si>
+    <t>["^Monster_schelp.*"]</t>
+  </si>
+  <si>
+    <t>["^Monster_botanie.*"]</t>
+  </si>
+  <si>
+    <t>["^R_DEEL"]</t>
+  </si>
+  <si>
+    <t>["^R_PLANT"]</t>
+  </si>
+  <si>
+    <t>["^R_SCHELP"]</t>
+  </si>
+  <si>
+    <t>["^R_STAAT"]</t>
   </si>
 </sst>
 </file>
@@ -3301,10 +3383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3334,7 +3416,7 @@
         <v>577</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -3378,7 +3460,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -3483,10 +3565,10 @@
         <v>19</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="H14" t="s">
         <v>578</v>
@@ -3506,10 +3588,10 @@
         <v>19</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="H15" t="s">
         <v>579</v>
@@ -3529,7 +3611,7 @@
         <v>19</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="H16" t="s">
         <v>580</v>
@@ -3549,10 +3631,10 @@
         <v>19</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="H17" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -3569,7 +3651,7 @@
         <v>19</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="H18" t="s">
         <v>581</v>
@@ -3589,7 +3671,7 @@
         <v>19</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="H19" t="s">
         <v>582</v>
@@ -3609,7 +3691,7 @@
         <v>19</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="H20" t="s">
         <v>582</v>
@@ -3629,10 +3711,10 @@
         <v>19</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="H21" t="s">
         <v>583</v>
@@ -3652,10 +3734,10 @@
         <v>19</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="H22" t="s">
         <v>585</v>
@@ -3675,10 +3757,10 @@
         <v>19</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="H23" t="s">
         <v>590</v>
@@ -3698,10 +3780,10 @@
         <v>19</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="H24" t="s">
         <v>588</v>
@@ -3721,10 +3803,10 @@
         <v>19</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="H25" t="s">
         <v>591</v>
@@ -3738,7 +3820,7 @@
         <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="D26" t="s">
         <v>19</v>
@@ -3761,10 +3843,10 @@
         <v>19</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="H27" t="s">
         <v>593</v>
@@ -3786,10 +3868,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C29" t="s">
-        <v>635</v>
+        <v>918</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -3797,10 +3879,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C30" t="s">
-        <v>637</v>
+        <v>919</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -3808,10 +3890,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="C31" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -3819,10 +3901,42 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="C32" t="s">
-        <v>890</v>
+        <v>887</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>897</v>
+      </c>
+      <c r="C33" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>898</v>
+      </c>
+      <c r="C34" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B35" s="7" t="s">
+        <v>899</v>
+      </c>
+      <c r="C35" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B36" s="7" t="s">
+        <v>900</v>
+      </c>
+      <c r="C36" t="s">
+        <v>923</v>
       </c>
     </row>
   </sheetData>
@@ -3855,6 +3969,323 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9079731B-8649-5A4E-B897-2AEB2B334294}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>610</v>
+      </c>
+      <c r="C2" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>896</v>
+      </c>
+      <c r="C4" t="s">
+        <v>625</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D386E297-D519-564E-ABC1-4EF5CC592387}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>610</v>
+      </c>
+      <c r="C2" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>895</v>
+      </c>
+      <c r="C3" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>626</v>
+      </c>
+      <c r="C4" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>628</v>
+      </c>
+      <c r="C5" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>630</v>
+      </c>
+      <c r="C6" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C7" t="s">
+        <v>632</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView zoomScale="270" zoomScaleNormal="270" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView zoomScale="230" zoomScaleNormal="230" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
@@ -4184,7 +4615,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
@@ -4507,7 +4938,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
@@ -4695,7 +5126,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -4738,11 +5169,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -4786,7 +5217,7 @@
         <v>185</v>
       </c>
       <c r="C3" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4899,7 +5330,7 @@
         <v>604</v>
       </c>
       <c r="C13" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4910,7 +5341,7 @@
         <v>605</v>
       </c>
       <c r="C14" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -5136,7 +5567,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="C35" t="s">
         <v>227</v>
@@ -5161,7 +5592,7 @@
         <v>230</v>
       </c>
       <c r="C37" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -5225,7 +5656,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -5432,7 +5863,129 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74421891-09E4-9B46-A9EF-46191FFB77E0}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>827</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>901</v>
+      </c>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>902</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>916</v>
+      </c>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>903</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>915</v>
+      </c>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>917</v>
+      </c>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="10"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -5551,7 +6104,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
@@ -5857,7 +6410,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -5888,7 +6441,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
@@ -6022,204 +6575,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22C687B-D5EB-1F49-BC93-522FCCA29282}">
-  <dimension ref="A1:D15"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>863</v>
-      </c>
-      <c r="C2" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <f>A2+1</f>
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>250</v>
-      </c>
-      <c r="C3" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <f t="shared" ref="A4:A15" si="0">A3+1</f>
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>867</v>
-      </c>
-      <c r="C4" t="s">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>868</v>
-      </c>
-      <c r="C5" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>889</v>
-      </c>
-      <c r="C6" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>871</v>
-      </c>
-      <c r="C7" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>873</v>
-      </c>
-      <c r="C8" t="s">
-        <v>888</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>874</v>
-      </c>
-      <c r="C9" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>876</v>
-      </c>
-      <c r="C10" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>878</v>
-      </c>
-      <c r="C11" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>880</v>
-      </c>
-      <c r="C12" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>882</v>
-      </c>
-      <c r="C13" t="s">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>884</v>
-      </c>
-      <c r="C14" t="s">
-        <v>885</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>886</v>
-      </c>
-      <c r="C15" t="s">
-        <v>887</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="B1:D1"/>
   <sheetViews>
@@ -6243,7 +6599,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D30"/>
   <sheetViews>
@@ -6588,7 +6944,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
@@ -6915,7 +7271,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
@@ -7130,7 +7486,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -7330,7 +7686,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
@@ -7629,7 +7985,123 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D10FD95C-4E22-A546-AFCF-A74850D837A1}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>827</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>905</v>
+      </c>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>903</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>914</v>
+      </c>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>906</v>
+      </c>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>907</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>908</v>
+      </c>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="10"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
@@ -7846,7 +8318,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC0267F-3961-F64D-889C-497261B556CC}">
   <dimension ref="B1:D12"/>
   <sheetViews>
@@ -7964,7 +8436,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71D0D174-6E0A-4C40-A400-825ECAC5A597}">
   <dimension ref="B1:D4"/>
   <sheetViews>
@@ -8019,12 +8491,208 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3BE5099-14EB-8E48-A984-D6BE092CC4FE}">
-  <dimension ref="A1:D100"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AE50202-C0E6-4F47-B457-2B64EBBADF5B}">
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection sqref="A1:D6"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>827</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>909</v>
+      </c>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>561</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>910</v>
+      </c>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>911</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>912</v>
+      </c>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC76FDFC-854B-EA4C-AF60-154B4D29E7EA}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>827</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>913</v>
+      </c>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>561</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>910</v>
+      </c>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="10"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22C687B-D5EB-1F49-BC93-522FCCA29282}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8049,10 +8717,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>860</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>861</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8061,22 +8729,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>250</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>862</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A67" si="0">A3+1</f>
+        <f t="shared" ref="A4:A15" si="0">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>864</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>863</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -8085,10 +8753,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>865</v>
       </c>
       <c r="C5" t="s">
-        <v>609</v>
+        <v>866</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -8097,10 +8765,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>610</v>
+        <v>886</v>
       </c>
       <c r="C6" t="s">
-        <v>611</v>
+        <v>867</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -8109,10 +8777,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>171</v>
+        <v>868</v>
       </c>
       <c r="C7" t="s">
-        <v>612</v>
+        <v>869</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -8121,10 +8789,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>613</v>
+        <v>870</v>
       </c>
       <c r="C8" t="s">
-        <v>614</v>
+        <v>885</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -8133,10 +8801,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>171</v>
+        <v>871</v>
       </c>
       <c r="C9" t="s">
-        <v>612</v>
+        <v>872</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -8145,10 +8813,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>873</v>
       </c>
       <c r="C10" t="s">
-        <v>615</v>
+        <v>874</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -8157,10 +8825,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>138</v>
+        <v>875</v>
       </c>
       <c r="C11" t="s">
-        <v>616</v>
+        <v>876</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -8169,10 +8837,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>617</v>
+        <v>877</v>
       </c>
       <c r="C12" t="s">
-        <v>618</v>
+        <v>878</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -8181,10 +8849,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>642</v>
+        <v>879</v>
       </c>
       <c r="C13" t="s">
-        <v>641</v>
+        <v>880</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -8193,10 +8861,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>643</v>
+        <v>881</v>
       </c>
       <c r="C14" t="s">
-        <v>644</v>
+        <v>882</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -8205,1033 +8873,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>619</v>
+        <v>883</v>
       </c>
       <c r="C15" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>213</v>
-      </c>
-      <c r="C16" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>622</v>
-      </c>
-      <c r="C17" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>638</v>
-      </c>
-      <c r="C18" t="s">
-        <v>639</v>
-      </c>
-      <c r="D18" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>645</v>
-      </c>
-      <c r="C19" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>646</v>
-      </c>
-      <c r="C20" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>647</v>
-      </c>
-      <c r="C21" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>648</v>
-      </c>
-      <c r="C22" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>649</v>
-      </c>
-      <c r="C23" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>650</v>
-      </c>
-      <c r="C24" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>651</v>
-      </c>
-      <c r="C25" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>652</v>
-      </c>
-      <c r="C26" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>661</v>
-      </c>
-      <c r="C27" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>785</v>
-      </c>
-      <c r="C28" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>786</v>
-      </c>
-      <c r="C29" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>787</v>
-      </c>
-      <c r="C30" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>788</v>
-      </c>
-      <c r="C31" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>667</v>
-      </c>
-      <c r="C32" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
-        <v>669</v>
-      </c>
-      <c r="C33" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
-        <v>671</v>
-      </c>
-      <c r="C34" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>673</v>
-      </c>
-      <c r="C35" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="B36" t="s">
-        <v>675</v>
-      </c>
-      <c r="C36" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
-        <v>677</v>
-      </c>
-      <c r="C37" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="B38" t="s">
-        <v>679</v>
-      </c>
-      <c r="C38" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="B39" t="s">
-        <v>681</v>
-      </c>
-      <c r="C39" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="B40" t="s">
-        <v>683</v>
-      </c>
-      <c r="C40" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="B41" t="s">
-        <v>685</v>
-      </c>
-      <c r="C41" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="B42" t="s">
-        <v>687</v>
-      </c>
-      <c r="C42" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="1">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="B43" t="s">
-        <v>689</v>
-      </c>
-      <c r="C43" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="B44" t="s">
-        <v>691</v>
-      </c>
-      <c r="C44" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="B45" t="s">
-        <v>789</v>
-      </c>
-      <c r="C45" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="1">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="B46" t="s">
-        <v>790</v>
-      </c>
-      <c r="C46" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="1">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="B47" t="s">
-        <v>803</v>
-      </c>
-      <c r="C47" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="1">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="B48" t="s">
-        <v>696</v>
-      </c>
-      <c r="C48" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="1">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="B49" t="s">
-        <v>804</v>
-      </c>
-      <c r="C49" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="1">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="B50" t="s">
-        <v>699</v>
-      </c>
-      <c r="C50" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="B51" t="s">
-        <v>701</v>
-      </c>
-      <c r="C51" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="1">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="B52" t="s">
-        <v>791</v>
-      </c>
-      <c r="C52" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="1">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="B53" t="s">
-        <v>704</v>
-      </c>
-      <c r="C53" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="1">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="B54" t="s">
-        <v>706</v>
-      </c>
-      <c r="C54" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="1">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="B55" t="s">
-        <v>708</v>
-      </c>
-      <c r="C55" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="1">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="B56" t="s">
-        <v>805</v>
-      </c>
-      <c r="C56" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="1">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="B57" t="s">
-        <v>711</v>
-      </c>
-      <c r="C57" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="1">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="B58" t="s">
-        <v>713</v>
-      </c>
-      <c r="C58" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="1">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="B59" t="s">
-        <v>715</v>
-      </c>
-      <c r="C59" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="1">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="B60" t="s">
-        <v>717</v>
-      </c>
-      <c r="C60" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="1">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="B61" t="s">
-        <v>719</v>
-      </c>
-      <c r="C61" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="1">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="B62" t="s">
-        <v>721</v>
-      </c>
-      <c r="C62" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="1">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
-      <c r="B63" t="s">
-        <v>723</v>
-      </c>
-      <c r="C63" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="1">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-      <c r="B64" t="s">
-        <v>725</v>
-      </c>
-      <c r="C64" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="1">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="B65" t="s">
-        <v>727</v>
-      </c>
-      <c r="C65" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="1">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="B66" t="s">
-        <v>792</v>
-      </c>
-      <c r="C66" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="1">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="B67" t="s">
-        <v>793</v>
-      </c>
-      <c r="C67" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="1">
-        <f t="shared" ref="A68:A100" si="1">A67+1</f>
-        <v>66</v>
-      </c>
-      <c r="B68" t="s">
-        <v>794</v>
-      </c>
-      <c r="C68" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="1">
-        <f t="shared" si="1"/>
-        <v>67</v>
-      </c>
-      <c r="B69" t="s">
-        <v>795</v>
-      </c>
-      <c r="C69" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="1">
-        <f t="shared" si="1"/>
-        <v>68</v>
-      </c>
-      <c r="B70" t="s">
-        <v>796</v>
-      </c>
-      <c r="C70" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="1">
-        <f t="shared" si="1"/>
-        <v>69</v>
-      </c>
-      <c r="B71" t="s">
-        <v>797</v>
-      </c>
-      <c r="C71" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="1">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="B72" t="s">
-        <v>798</v>
-      </c>
-      <c r="C72" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="1">
-        <f t="shared" si="1"/>
-        <v>71</v>
-      </c>
-      <c r="B73" t="s">
-        <v>799</v>
-      </c>
-      <c r="C73" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="1">
-        <f t="shared" si="1"/>
-        <v>72</v>
-      </c>
-      <c r="B74" t="s">
-        <v>737</v>
-      </c>
-      <c r="C74" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="1">
-        <f t="shared" si="1"/>
-        <v>73</v>
-      </c>
-      <c r="B75" t="s">
-        <v>739</v>
-      </c>
-      <c r="C75" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="1">
-        <f t="shared" si="1"/>
-        <v>74</v>
-      </c>
-      <c r="B76" t="s">
-        <v>741</v>
-      </c>
-      <c r="C76" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="1">
-        <f t="shared" si="1"/>
-        <v>75</v>
-      </c>
-      <c r="B77" t="s">
-        <v>743</v>
-      </c>
-      <c r="C77" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="1">
-        <f t="shared" si="1"/>
-        <v>76</v>
-      </c>
-      <c r="B78" t="s">
-        <v>745</v>
-      </c>
-      <c r="C78" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="1">
-        <f t="shared" si="1"/>
-        <v>77</v>
-      </c>
-      <c r="B79" t="s">
-        <v>747</v>
-      </c>
-      <c r="C79" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="1">
-        <f t="shared" si="1"/>
-        <v>78</v>
-      </c>
-      <c r="B80" t="s">
-        <v>749</v>
-      </c>
-      <c r="C80" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="1">
-        <f t="shared" si="1"/>
-        <v>79</v>
-      </c>
-      <c r="B81" t="s">
-        <v>751</v>
-      </c>
-      <c r="C81" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="1">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="B82" t="s">
-        <v>753</v>
-      </c>
-      <c r="C82" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="1">
-        <f t="shared" si="1"/>
-        <v>81</v>
-      </c>
-      <c r="B83" t="s">
-        <v>755</v>
-      </c>
-      <c r="C83" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="1">
-        <f t="shared" si="1"/>
-        <v>82</v>
-      </c>
-      <c r="B84" t="s">
-        <v>806</v>
-      </c>
-      <c r="C84" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="1">
-        <f t="shared" si="1"/>
-        <v>83</v>
-      </c>
-      <c r="B85" t="s">
-        <v>758</v>
-      </c>
-      <c r="C85" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="1">
-        <f t="shared" si="1"/>
-        <v>84</v>
-      </c>
-      <c r="B86" t="s">
-        <v>760</v>
-      </c>
-      <c r="C86" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="1">
-        <f t="shared" si="1"/>
-        <v>85</v>
-      </c>
-      <c r="B87" t="s">
-        <v>762</v>
-      </c>
-      <c r="C87" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="1">
-        <f t="shared" si="1"/>
-        <v>86</v>
-      </c>
-      <c r="B88" t="s">
-        <v>764</v>
-      </c>
-      <c r="C88" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" s="1">
-        <f t="shared" si="1"/>
-        <v>87</v>
-      </c>
-      <c r="B89" t="s">
-        <v>800</v>
-      </c>
-      <c r="C89" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" s="1">
-        <f t="shared" si="1"/>
-        <v>88</v>
-      </c>
-      <c r="B90" t="s">
-        <v>801</v>
-      </c>
-      <c r="C90" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" s="1">
-        <f t="shared" si="1"/>
-        <v>89</v>
-      </c>
-      <c r="B91" t="s">
-        <v>807</v>
-      </c>
-      <c r="C91" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="1">
-        <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-      <c r="B92" t="s">
-        <v>769</v>
-      </c>
-      <c r="C92" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" s="1">
-        <f t="shared" si="1"/>
-        <v>91</v>
-      </c>
-      <c r="B93" t="s">
-        <v>808</v>
-      </c>
-      <c r="C93" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94" s="1">
-        <f t="shared" si="1"/>
-        <v>92</v>
-      </c>
-      <c r="B94" t="s">
-        <v>772</v>
-      </c>
-      <c r="C94" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95" s="1">
-        <f t="shared" si="1"/>
-        <v>93</v>
-      </c>
-      <c r="B95" t="s">
-        <v>774</v>
-      </c>
-      <c r="C95" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" s="1">
-        <f t="shared" si="1"/>
-        <v>94</v>
-      </c>
-      <c r="B96" t="s">
-        <v>776</v>
-      </c>
-      <c r="C96" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" s="1">
-        <f t="shared" si="1"/>
-        <v>95</v>
-      </c>
-      <c r="B97" t="s">
-        <v>778</v>
-      </c>
-      <c r="C97" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" s="1">
-        <f t="shared" si="1"/>
-        <v>96</v>
-      </c>
-      <c r="B98" t="s">
-        <v>780</v>
-      </c>
-      <c r="C98" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" s="1">
-        <f t="shared" si="1"/>
-        <v>97</v>
-      </c>
-      <c r="B99" t="s">
-        <v>802</v>
-      </c>
-      <c r="C99" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A100" s="1">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-      <c r="B100" t="s">
-        <v>783</v>
-      </c>
-      <c r="C100" t="s">
-        <v>784</v>
+        <v>884</v>
       </c>
     </row>
   </sheetData>
@@ -9239,7 +8884,1227 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3BE5099-14EB-8E48-A984-D6BE092CC4FE}">
+  <dimension ref="A1:D100"/>
+  <sheetViews>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <f t="shared" ref="A4:A67" si="0">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>610</v>
+      </c>
+      <c r="C6" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C7" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>613</v>
+      </c>
+      <c r="C8" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C9" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C11" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>617</v>
+      </c>
+      <c r="C12" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>639</v>
+      </c>
+      <c r="C13" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>640</v>
+      </c>
+      <c r="C14" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>619</v>
+      </c>
+      <c r="C15" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>213</v>
+      </c>
+      <c r="C16" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>622</v>
+      </c>
+      <c r="C17" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>635</v>
+      </c>
+      <c r="C18" t="s">
+        <v>636</v>
+      </c>
+      <c r="D18" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>642</v>
+      </c>
+      <c r="C19" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>643</v>
+      </c>
+      <c r="C20" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>644</v>
+      </c>
+      <c r="C21" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>645</v>
+      </c>
+      <c r="C22" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>646</v>
+      </c>
+      <c r="C23" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>647</v>
+      </c>
+      <c r="C24" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>648</v>
+      </c>
+      <c r="C25" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>649</v>
+      </c>
+      <c r="C26" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>658</v>
+      </c>
+      <c r="C27" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>782</v>
+      </c>
+      <c r="C28" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>783</v>
+      </c>
+      <c r="C29" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>784</v>
+      </c>
+      <c r="C30" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>785</v>
+      </c>
+      <c r="C31" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>664</v>
+      </c>
+      <c r="C32" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>666</v>
+      </c>
+      <c r="C33" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>668</v>
+      </c>
+      <c r="C34" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>670</v>
+      </c>
+      <c r="C35" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>672</v>
+      </c>
+      <c r="C36" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>674</v>
+      </c>
+      <c r="C37" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>676</v>
+      </c>
+      <c r="C38" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>678</v>
+      </c>
+      <c r="C39" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>680</v>
+      </c>
+      <c r="C40" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>682</v>
+      </c>
+      <c r="C41" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>684</v>
+      </c>
+      <c r="C42" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>686</v>
+      </c>
+      <c r="C43" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>688</v>
+      </c>
+      <c r="C44" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>786</v>
+      </c>
+      <c r="C45" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>787</v>
+      </c>
+      <c r="C46" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>800</v>
+      </c>
+      <c r="C47" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>693</v>
+      </c>
+      <c r="C48" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>801</v>
+      </c>
+      <c r="C49" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>696</v>
+      </c>
+      <c r="C50" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>698</v>
+      </c>
+      <c r="C51" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>788</v>
+      </c>
+      <c r="C52" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>701</v>
+      </c>
+      <c r="C53" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>703</v>
+      </c>
+      <c r="C54" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>705</v>
+      </c>
+      <c r="C55" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>802</v>
+      </c>
+      <c r="C56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>708</v>
+      </c>
+      <c r="C57" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>710</v>
+      </c>
+      <c r="C58" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>712</v>
+      </c>
+      <c r="C59" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>714</v>
+      </c>
+      <c r="C60" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>716</v>
+      </c>
+      <c r="C61" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>718</v>
+      </c>
+      <c r="C62" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>720</v>
+      </c>
+      <c r="C63" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>722</v>
+      </c>
+      <c r="C64" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>724</v>
+      </c>
+      <c r="C65" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>789</v>
+      </c>
+      <c r="C66" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>790</v>
+      </c>
+      <c r="C67" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <f t="shared" ref="A68:A100" si="1">A67+1</f>
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>791</v>
+      </c>
+      <c r="C68" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>792</v>
+      </c>
+      <c r="C69" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>793</v>
+      </c>
+      <c r="C70" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>794</v>
+      </c>
+      <c r="C71" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>795</v>
+      </c>
+      <c r="C72" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>796</v>
+      </c>
+      <c r="C73" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>734</v>
+      </c>
+      <c r="C74" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>736</v>
+      </c>
+      <c r="C75" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>738</v>
+      </c>
+      <c r="C76" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>740</v>
+      </c>
+      <c r="C77" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
+        <v>742</v>
+      </c>
+      <c r="C78" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>744</v>
+      </c>
+      <c r="C79" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="B80" t="s">
+        <v>746</v>
+      </c>
+      <c r="C80" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>748</v>
+      </c>
+      <c r="C81" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="B82" t="s">
+        <v>750</v>
+      </c>
+      <c r="C82" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="B83" t="s">
+        <v>752</v>
+      </c>
+      <c r="C83" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
+        <v>803</v>
+      </c>
+      <c r="C84" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="B85" t="s">
+        <v>755</v>
+      </c>
+      <c r="C85" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="B86" t="s">
+        <v>757</v>
+      </c>
+      <c r="C86" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
+        <v>759</v>
+      </c>
+      <c r="C87" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>761</v>
+      </c>
+      <c r="C88" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="B89" t="s">
+        <v>797</v>
+      </c>
+      <c r="C89" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="B90" t="s">
+        <v>798</v>
+      </c>
+      <c r="C90" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="B91" t="s">
+        <v>804</v>
+      </c>
+      <c r="C91" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>766</v>
+      </c>
+      <c r="C92" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>805</v>
+      </c>
+      <c r="C93" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
+        <v>769</v>
+      </c>
+      <c r="C94" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="B95" t="s">
+        <v>771</v>
+      </c>
+      <c r="C95" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="B96" t="s">
+        <v>773</v>
+      </c>
+      <c r="C96" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="B97" t="s">
+        <v>775</v>
+      </c>
+      <c r="C97" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="B98" t="s">
+        <v>777</v>
+      </c>
+      <c r="C98" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
+        <v>799</v>
+      </c>
+      <c r="C99" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
+        <v>780</v>
+      </c>
+      <c r="C100" t="s">
+        <v>781</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3031EEAA-8CBE-224C-882A-D80708C8602F}">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -9270,10 +10135,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="D2" s="7"/>
     </row>
@@ -9283,10 +10148,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="D3" s="7"/>
     </row>
@@ -9296,10 +10161,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="D4" s="7"/>
     </row>
@@ -9309,10 +10174,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="D5" s="7"/>
     </row>
@@ -9322,10 +10187,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="D6" s="7"/>
     </row>
@@ -9335,10 +10200,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="D7" s="7"/>
     </row>
@@ -9348,10 +10213,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="D8" s="7"/>
     </row>
@@ -9361,10 +10226,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="D9" s="7"/>
     </row>
@@ -9377,7 +10242,7 @@
         <v>213</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="D10" s="7"/>
     </row>
@@ -9387,10 +10252,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="D11" s="7"/>
     </row>
@@ -9400,10 +10265,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="D12" s="7"/>
     </row>
@@ -9412,7 +10277,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF775CC9-C6C8-ED4F-B48D-81639A81E38C}">
   <dimension ref="A1:D15"/>
   <sheetViews>
@@ -9440,10 +10305,10 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="7" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="D2" s="11"/>
     </row>
@@ -9500,10 +10365,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="D7" s="7"/>
     </row>
@@ -9512,23 +10377,23 @@
         <v>168</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -9536,15 +10401,15 @@
         <v>561</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -9552,343 +10417,26 @@
         <v>103</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="7" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9079731B-8649-5A4E-B897-2AEB2B334294}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>610</v>
-      </c>
-      <c r="C2" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C3" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>625</v>
-      </c>
-      <c r="C4" t="s">
-        <v>626</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D386E297-D519-564E-ABC1-4EF5CC592387}">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>610</v>
-      </c>
-      <c r="C2" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>625</v>
-      </c>
-      <c r="C3" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C4" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>629</v>
-      </c>
-      <c r="C5" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>631</v>
-      </c>
-      <c r="C6" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>185</v>
-      </c>
-      <c r="C7" t="s">
-        <v>633</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView zoomScale="270" zoomScaleNormal="270" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView zoomScale="230" zoomScaleNormal="230" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>